<commit_message>
Update Col Mapping with Fairfield Licking
</commit_message>
<xml_diff>
--- a/docs/Column mapping.xlsx
+++ b/docs/Column mapping.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cullimk/Documents/pers/Data Analytics/WIIT 7110 Applied Data Analytics/Group Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F24EAA5B-3D92-A14F-84C4-33C74F7A133D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{39A98C95-0433-7444-8B84-1505545765D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26940" yWindow="3100" windowWidth="25440" windowHeight="13000"/>
+    <workbookView xWindow="18800" yWindow="460" windowWidth="10000" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="268" uniqueCount="197">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="600" uniqueCount="510">
   <si>
     <t>Parcel</t>
   </si>
@@ -616,13 +621,952 @@
   </si>
   <si>
     <t>Thought we could do tax (purple), but the values in Madison file don't seem to be equivalent to Annual Tax like Morrow/Franklin</t>
+  </si>
+  <si>
+    <t>Franklin (WebReporter)</t>
+  </si>
+  <si>
+    <t>Parcel Number</t>
+  </si>
+  <si>
+    <t>Site Address</t>
+  </si>
+  <si>
+    <t>Acres (GIS Calculated)</t>
+  </si>
+  <si>
+    <t>Legal Description 1</t>
+  </si>
+  <si>
+    <t>Legal Description 2</t>
+  </si>
+  <si>
+    <t>Legal Description 3</t>
+  </si>
+  <si>
+    <t>Neighborhood</t>
+  </si>
+  <si>
+    <t>Owner Name 1</t>
+  </si>
+  <si>
+    <t>Owner Name 2</t>
+  </si>
+  <si>
+    <t>Tax Mailing Address 1</t>
+  </si>
+  <si>
+    <t>Tax Mailing Address 2</t>
+  </si>
+  <si>
+    <t>Tax Mailing Address 3</t>
+  </si>
+  <si>
+    <t>Tax Mailing Address 4</t>
+  </si>
+  <si>
+    <t>Primary Land Use Code</t>
+  </si>
+  <si>
+    <t>Sale Date</t>
+  </si>
+  <si>
+    <t>Sale Price</t>
+  </si>
+  <si>
+    <t>Year Built</t>
+  </si>
+  <si>
+    <t>Total Rooms</t>
+  </si>
+  <si>
+    <t>Bedrooms</t>
+  </si>
+  <si>
+    <t>Full Baths</t>
+  </si>
+  <si>
+    <t>Half Baths</t>
+  </si>
+  <si>
+    <t>Area Finished Above Grade</t>
+  </si>
+  <si>
+    <t>Area Finished Below Grade</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>TotalBaths</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>County (ADDED)</t>
+  </si>
+  <si>
+    <t>=drop</t>
+  </si>
+  <si>
+    <t>Acres                float64</t>
+  </si>
+  <si>
+    <t>County                object</t>
+  </si>
+  <si>
+    <t>FinishedArea         float64</t>
+  </si>
+  <si>
+    <t>LandUse              float64</t>
+  </si>
+  <si>
+    <t>LegalDescription      object</t>
+  </si>
+  <si>
+    <t>MailingAddress        object</t>
+  </si>
+  <si>
+    <t>NeighborhoodCode      object</t>
+  </si>
+  <si>
+    <t>NumberOfBedrooms     float64</t>
+  </si>
+  <si>
+    <t>NumberOfRooms        float64</t>
+  </si>
+  <si>
+    <t>Owner                 object</t>
+  </si>
+  <si>
+    <t>Parcel                object</t>
+  </si>
+  <si>
+    <t>PropertyAddress       object</t>
+  </si>
+  <si>
+    <t>SaleDate              object</t>
+  </si>
+  <si>
+    <t>SalePrice            float64</t>
+  </si>
+  <si>
+    <t>YearBuilt             object</t>
+  </si>
+  <si>
+    <t>float64</t>
+  </si>
+  <si>
+    <t>'PIN',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Shape_Leng',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Shape_Area',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'PARID',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'OWN1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'OWN2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LASTNAME',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ADRNO',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ADRDIR',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ADRSTR',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ADRSUF',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ADRSUF2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'PADDR1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'MADDR1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'MADDR2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'MADDR3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'MCITYNAME',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'MSTATECODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'MZIP1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LEGAL1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LEGAL2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LEGAL3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ACRES',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'MAPNUM',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ROUTENUM',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LUC',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'PARTIAL_',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'NBHD',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'STORIES',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'EXTWALL',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'STYLE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'SFLA',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'YRBLT',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'YRREMOD',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'RMTOT',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'RMBED',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'RMFAM',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FIXBATH',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FIXHALF',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FIXTOT',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BSMT',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'HEAT',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FUEL',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ATTIC',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'WBFP_O',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'WBFP_S',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'WBFP_PF',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BSMTCAR',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FINBSMTARE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'RECROMAREA',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'MASTRIMARE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BOOK',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'PAGE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'SALEDT',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TRANSDT',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'RECORDDT',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'PRICE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'SALEVAL',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'SALETYPE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'APRLAND',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'APRBLDG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FARMLAND',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'AGAPPL',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'SALEYEAR',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'APPRVAL',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'SALESRATIO',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'GRDFACT',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'CDU',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'CLASS',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'DEPR',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'geometry'</t>
+  </si>
+  <si>
+    <t>Fairfield</t>
+  </si>
+  <si>
+    <t>**Missing Landuse Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldParcelNo',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldRoutingNo',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldOwner',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCardNo',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMaxCards',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldRecheck',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSchoolDistrict',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldTaxDistrict',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldLegalDesc',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldLocationAddress',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldNeighborhood',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldPropertyType',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldLUC',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldTopo',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAccess',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldUtilities',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldNotes',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldNotes2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMarketLand',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMarketImprov',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMarketTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCAUVLand',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCAUVImprov',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCAUVTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSketchPath',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldStyle',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldStories',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldExterior',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldHeating',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCooling',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldBasement',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFullBaths',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldHalfBaths',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldOtherBaths',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAttic',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAtticHeating',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldRooms',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldBedrooms',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFamilyRooms',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldDiningRooms',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldLivingRooms',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFinishedLivingArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFinishedBasementArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldYearBuilt',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldEffYearBuilt',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldYearRemodeled',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCondition',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldGrade',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldBasementGarage',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFireplaceOpenings',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFireplaceStacks',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFirstFloorArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFirstFloorCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldUpperFloorArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldUpperFloorCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAtticArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAtticCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldHalfFloorArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldHalfFloorCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFinishedBasementCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldUnfinishedLivingArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldUnfinishedLivingCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCrawlArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCrawlCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldBasementArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldBasementCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldBasementGarageArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldBasementGarageCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldExtWallArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldExtWallCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldHeatingArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldHeatingCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCoolingArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCoolingCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldPlumbingArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldPlumbingCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFireplaceArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFireplaceCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldIdenticalMultiplierCount',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldIdenticalMultiplierCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldEnhancementArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldEnhancementCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFeaturesArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFeaturesCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSubTotalBeforeGrade',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldGradeArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldGradeCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCostFactorArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCostFactorCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldUngradedFeaturesArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldUngradedFeaturesCost',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldRCN',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldDepreciation',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldDepreciationOverride',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldDepreciationArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldObsolesence',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldObsolesenceArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldImprovements',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldRCNLD',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldImprovementsTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFVC',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldWellSeptic',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldWellSepticValue',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryYear1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryYear2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryYear3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryLand1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryLand2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryLand3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryImprov1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryImprov2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryImprov3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryTotal1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryTotal2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldValueHistoryTotal3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesDate1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesDate2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesDate3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesDate4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesNoParcels1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesNoParcels2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesNoParcels3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesNoParcels4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesType1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesType2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesType3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesType4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesPrice1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesPrice2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesPrice3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesPrice4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesConveyance1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesConveyance2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesConveyance3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesConveyance4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesValid1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesValid2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesValid3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesValid4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesLandOnly1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesLandOnly2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesLandOnly3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesLandOnly4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesPrevOwner1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesPrevOwner2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesPrevOwner3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSalesPrevOwner4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldFeatureTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldLandTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldImprovTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldEnhancementTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldTaxYear',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSubtotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAdditionalInspections',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAdditionalEnhancements',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAdditionalFeatures',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAdditionalLand',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAdditionalImprovements',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldNeighAdj',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldNeighAdjArea',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCard1Total',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCard2Total',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCard3Total',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCard4Total',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCard5Total',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldParcelTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldPicPath',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldAcreageTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldSortOrder',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldCropTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldWoodsTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldNotFarmedTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldConservationTotal',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldNeighAdjLandOverride',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldNeighAdjAreaLand',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHYear',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHMake',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHModel',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHPark',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHAquisition',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHSize',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHPrice',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHSitus',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHCertNumber',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHSerialNumber',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHRealParcel',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHDeprTaxable',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMHDeprValue',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMailingAddress1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMailingAddress2',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMailingAddress3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMailingAddress4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fldMailingAddress5'</t>
+  </si>
+  <si>
+    <t>Licking</t>
+  </si>
+  <si>
+    <t>fldParcelID',</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -762,6 +1706,12 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="51">
     <fill>
@@ -1041,13 +1991,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1212,7 +2162,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1232,9 +2182,31 @@
     <xf numFmtId="0" fontId="17" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1589,980 +2561,2292 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G76"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="64" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="12" width="28" customWidth="1"/>
+    <col min="13" max="13" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13">
+      <c r="B1" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="M1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="24"/>
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>108</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>509</v>
+      </c>
+      <c r="M2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:13" ht="19">
+      <c r="B3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>109</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="L3" s="37" t="s">
+        <v>315</v>
+      </c>
+      <c r="M3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:13" ht="19">
+      <c r="B4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>110</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>316</v>
+      </c>
+      <c r="M4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:13">
+      <c r="B5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>57</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>111</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:13" ht="19">
+      <c r="A6" s="24"/>
+      <c r="B6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>58</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
         <v>112</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L6" s="37" t="s">
+        <v>318</v>
+      </c>
+      <c r="M6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:13" ht="19">
+      <c r="B7" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="31"/>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>59</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>113</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="L7" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="M7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:13" ht="19">
+      <c r="B8" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>60</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>60</v>
       </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
         <v>114</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>320</v>
+      </c>
+      <c r="M8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:13" ht="19">
+      <c r="B9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>61</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>61</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" t="s">
         <v>115</v>
       </c>
-      <c r="G9" t="s">
+      <c r="J9" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="L9" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="M9" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:13" ht="19">
+      <c r="A10" s="24"/>
+      <c r="B10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>62</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>62</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>116</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="L10" s="37" t="s">
+        <v>322</v>
+      </c>
+      <c r="M10" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:13">
+      <c r="A11" s="24"/>
+      <c r="B11" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="35"/>
+      <c r="D11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>63</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
         <v>63</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>117</v>
       </c>
-      <c r="G11" t="s">
+      <c r="J11" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="L11" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="M11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
+    <row r="12" spans="1:13">
+      <c r="A12" s="13"/>
+      <c r="B12" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="F12" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
         <v>118</v>
       </c>
-      <c r="G12" t="s">
+      <c r="J12" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="M12" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
         <v>64</v>
       </c>
-      <c r="E13" t="s">
+      <c r="H13" t="s">
         <v>64</v>
       </c>
-      <c r="F13" t="s">
+      <c r="I13" t="s">
         <v>119</v>
       </c>
-      <c r="G13" t="s">
+      <c r="J13" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="L13" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="M13" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
+    <row r="14" spans="1:13" ht="19">
+      <c r="B14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="s">
+      <c r="G14" t="s">
         <v>65</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>65</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="12" t="s">
+      <c r="J14" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="E15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
+      <c r="G15" t="s">
         <v>66</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
         <v>66</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="14" t="s">
+      <c r="J15" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="19">
+      <c r="B16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="F16" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I16" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="15" t="s">
+      <c r="J16" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="L16" s="37" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="19">
+      <c r="B17" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E17" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F17" t="s">
+      <c r="I17" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="16" t="s">
+      <c r="J17" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="L17" s="37" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="19">
+      <c r="B18" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F18" t="s">
+      <c r="I18" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
+      <c r="J18" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="L18" s="37" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="19">
+      <c r="D19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E19" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F19" t="s">
+      <c r="I19" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="J19" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="L19" s="37" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="19">
       <c r="A20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="G20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="H20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F20" t="s">
+      <c r="I20" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="17" t="s">
+      <c r="J20" t="s">
+        <v>215</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="L20" s="37" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="19">
+      <c r="D21" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="F21" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="H21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F21" t="s">
+      <c r="I21" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="17" t="s">
+      <c r="J21" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="K21" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="L21" s="37" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="19">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="E22" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F22" t="s">
+      <c r="I22" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="18" t="s">
+      <c r="J22" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="K22" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="L22" s="37" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="19">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="E23" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F23" t="s">
+      <c r="I23" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="J23" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="L23" s="37" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="19">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="D24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="E24" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
+      <c r="J24" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="K24" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="L24" s="37" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="19">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F25" t="s">
+      <c r="I25" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
+      <c r="J25" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="L25" s="37" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="19">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="E26" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="G26" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="H26" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F26" t="s">
+      <c r="I26" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
+      <c r="K26" t="s">
+        <v>266</v>
+      </c>
+      <c r="L26" s="37" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="19">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="D27" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="E27" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="F27" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="D27" t="s">
+      <c r="G27" t="s">
         <v>78</v>
       </c>
-      <c r="E27" t="s">
+      <c r="H27" t="s">
         <v>78</v>
       </c>
-      <c r="F27" t="s">
+      <c r="I27" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
+      <c r="K27" t="s">
+        <v>267</v>
+      </c>
+      <c r="L27" s="37" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="19">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="D28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="E28" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D28" t="s">
+      <c r="G28" t="s">
         <v>79</v>
       </c>
-      <c r="E28" t="s">
+      <c r="H28" t="s">
         <v>79</v>
       </c>
-      <c r="F28" t="s">
+      <c r="I28" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="19" t="s">
+      <c r="K28" t="s">
+        <v>268</v>
+      </c>
+      <c r="L28" s="37" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="19">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="D29" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="E29" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="6" t="s">
+      <c r="F29" s="19"/>
+      <c r="G29" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F29" t="s">
+      <c r="I29" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="B30" t="s">
+      <c r="K29" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="19">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="E30" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="G30" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="H30" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F30" t="s">
+      <c r="I30" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="B31" t="s">
+      <c r="K30" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="L30" s="37" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="19">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="E31" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="G31" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="H31" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F31" t="s">
+      <c r="I31" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="B32" s="17" t="s">
+      <c r="K31" t="s">
+        <v>271</v>
+      </c>
+      <c r="L31" s="37" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="19">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="3" t="s">
+      <c r="F32" s="19"/>
+      <c r="G32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F32" t="s">
+      <c r="I32" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" s="17" t="s">
+      <c r="K32" t="s">
+        <v>272</v>
+      </c>
+      <c r="L32" s="37" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="19">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="E33" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" t="s">
+      <c r="F33" s="19"/>
+      <c r="G33" t="s">
         <v>84</v>
       </c>
-      <c r="E33" t="s">
+      <c r="H33" t="s">
         <v>84</v>
       </c>
-      <c r="F33" t="s">
+      <c r="I33" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" s="14" t="s">
+      <c r="K33" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="L33" s="37" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="19">
+      <c r="A34">
+        <v>13</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D34" t="s">
+      <c r="F34" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G34" t="s">
         <v>85</v>
       </c>
-      <c r="E34" t="s">
+      <c r="H34" t="s">
         <v>85</v>
       </c>
-      <c r="F34" t="s">
+      <c r="I34" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" t="s">
+      <c r="K34" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="19">
+      <c r="A35">
+        <v>14</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="E35" t="s">
         <v>48</v>
       </c>
-      <c r="D35" t="s">
+      <c r="G35" t="s">
         <v>86</v>
       </c>
-      <c r="E35" t="s">
+      <c r="H35" t="s">
         <v>86</v>
       </c>
-      <c r="F35" t="s">
+      <c r="I35" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" t="s">
+      <c r="K35" t="s">
+        <v>275</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="19">
+      <c r="A36">
+        <v>15</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="E36" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="G36" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="H36" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F36" t="s">
+      <c r="I36" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="B37" t="s">
+      <c r="K36" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="L36" s="37" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="19">
+      <c r="A37">
+        <v>16</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="E37" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="G37" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="H37" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F37" t="s">
+      <c r="I37" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="B38" t="s">
+      <c r="K37" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="L37" s="37" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="19">
+      <c r="E38" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="G38" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="H38" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F38" t="s">
+      <c r="I38" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="B39" t="s">
+      <c r="K38" t="s">
+        <v>278</v>
+      </c>
+      <c r="L38" s="37" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="E39" t="s">
         <v>52</v>
       </c>
-      <c r="D39" t="s">
+      <c r="G39" t="s">
         <v>90</v>
       </c>
-      <c r="E39" t="s">
+      <c r="H39" t="s">
         <v>90</v>
       </c>
-      <c r="F39" t="s">
+      <c r="I39" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="B40" t="s">
+      <c r="K39" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="L39" s="15" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="E40" t="s">
         <v>53</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="G40" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="H40" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="F40" t="s">
+      <c r="I40" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="41" spans="2:6">
-      <c r="D41" t="s">
+      <c r="K40" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="19">
+      <c r="G41" t="s">
         <v>92</v>
       </c>
-      <c r="E41" t="s">
+      <c r="H41" t="s">
         <v>92</v>
       </c>
-      <c r="F41" t="s">
+      <c r="I41" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="D42" s="15" t="s">
+      <c r="K41" t="s">
+        <v>281</v>
+      </c>
+      <c r="L41" s="37" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="19">
+      <c r="G42" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="H42" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="F42" t="s">
+      <c r="I42" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="43" spans="2:6">
-      <c r="D43" s="17" t="s">
+      <c r="K42" t="s">
+        <v>282</v>
+      </c>
+      <c r="L42" s="37" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="19">
+      <c r="G43" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="H43" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F43" t="s">
+      <c r="I43" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="D44" s="17" t="s">
+      <c r="K43" t="s">
+        <v>283</v>
+      </c>
+      <c r="L43" s="37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="G44" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="H44" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F44" t="s">
+      <c r="I44" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="45" spans="2:6">
-      <c r="D45" s="16" t="s">
+      <c r="K44" t="s">
+        <v>284</v>
+      </c>
+      <c r="L44" s="14" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="19">
+      <c r="G45" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="H45" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="F45" t="s">
+      <c r="I45" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="46" spans="2:6">
-      <c r="D46" t="s">
+      <c r="K45" t="s">
+        <v>285</v>
+      </c>
+      <c r="L45" s="37" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="G46" t="s">
         <v>97</v>
       </c>
-      <c r="E46" t="s">
+      <c r="H46" t="s">
         <v>97</v>
       </c>
-      <c r="F46" t="s">
+      <c r="I46" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="47" spans="2:6">
-      <c r="D47" t="s">
+      <c r="K46" t="s">
+        <v>286</v>
+      </c>
+      <c r="L46" s="36" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="19">
+      <c r="G47" t="s">
         <v>98</v>
       </c>
-      <c r="E47" t="s">
+      <c r="H47" t="s">
         <v>98</v>
       </c>
-      <c r="F47" t="s">
+      <c r="I47" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="48" spans="2:6">
-      <c r="D48" t="s">
+      <c r="K47" t="s">
+        <v>287</v>
+      </c>
+      <c r="L47" s="37" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="19">
+      <c r="G48" t="s">
         <v>99</v>
       </c>
-      <c r="E48" t="s">
+      <c r="H48" t="s">
         <v>99</v>
       </c>
-      <c r="F48" t="s">
+      <c r="I48" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="49" spans="4:6">
-      <c r="D49" t="s">
+      <c r="K48" t="s">
+        <v>288</v>
+      </c>
+      <c r="L48" s="37" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="49" spans="7:12" ht="19">
+      <c r="G49" t="s">
         <v>100</v>
       </c>
-      <c r="E49" t="s">
+      <c r="H49" t="s">
         <v>100</v>
       </c>
-      <c r="F49" t="s">
+      <c r="I49" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="50" spans="4:6">
-      <c r="D50" s="13" t="s">
+      <c r="K49" t="s">
+        <v>289</v>
+      </c>
+      <c r="L49" s="37" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="50" spans="7:12" ht="19">
+      <c r="G50" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="13" t="s">
+      <c r="H50" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="F50" t="s">
+      <c r="I50" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="51" spans="4:6">
-      <c r="D51" s="12" t="s">
+      <c r="K50" t="s">
+        <v>290</v>
+      </c>
+      <c r="L50" s="37" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="51" spans="7:12" ht="19">
+      <c r="G51" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="H51" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="F51" t="s">
+      <c r="I51" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="52" spans="4:6">
-      <c r="D52" s="11" t="s">
+      <c r="K51" t="s">
+        <v>291</v>
+      </c>
+      <c r="L51" s="37" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="52" spans="7:12" ht="19">
+      <c r="G52" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="H52" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F52" t="s">
+      <c r="I52" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="53" spans="4:6">
-      <c r="D53" t="s">
+      <c r="K52" t="s">
+        <v>292</v>
+      </c>
+      <c r="L52" s="37" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="53" spans="7:12" ht="19">
+      <c r="G53" t="s">
         <v>104</v>
       </c>
-      <c r="E53" t="s">
+      <c r="H53" t="s">
         <v>104</v>
       </c>
-      <c r="F53" t="s">
+      <c r="I53" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="54" spans="4:6">
-      <c r="F54" t="s">
+      <c r="K53" t="s">
+        <v>293</v>
+      </c>
+      <c r="L53" s="37" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="54" spans="7:12" ht="19">
+      <c r="I54" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="55" spans="4:6">
-      <c r="F55" t="s">
+      <c r="K54" t="s">
+        <v>294</v>
+      </c>
+      <c r="L54" s="37" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="55" spans="7:12" ht="19">
+      <c r="I55" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="56" spans="4:6">
-      <c r="F56" t="s">
+      <c r="K55" s="34" t="s">
+        <v>295</v>
+      </c>
+      <c r="L55" s="37" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="56" spans="7:12" ht="19">
+      <c r="I56" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="57" spans="4:6">
-      <c r="F57" t="s">
+      <c r="K56" t="s">
+        <v>296</v>
+      </c>
+      <c r="L56" s="37" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="57" spans="7:12" ht="19">
+      <c r="I57" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="58" spans="4:6">
-      <c r="F58" t="s">
+      <c r="K57" t="s">
+        <v>297</v>
+      </c>
+      <c r="L57" s="37" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="58" spans="7:12" ht="19">
+      <c r="I58" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="59" spans="4:6">
-      <c r="F59" t="s">
+      <c r="K58" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="L58" s="37" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="59" spans="7:12" ht="19">
+      <c r="I59" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="60" spans="4:6">
-      <c r="F60" t="s">
+      <c r="K59" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="L59" s="37" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="60" spans="7:12" ht="19">
+      <c r="I60" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="61" spans="4:6">
-      <c r="F61" t="s">
+      <c r="K60" t="s">
+        <v>300</v>
+      </c>
+      <c r="L60" s="37" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="61" spans="7:12" ht="19">
+      <c r="I61" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="62" spans="4:6">
-      <c r="F62" t="s">
+      <c r="K61" t="s">
+        <v>301</v>
+      </c>
+      <c r="L61" s="37" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="62" spans="7:12" ht="19">
+      <c r="I62" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="63" spans="4:6">
-      <c r="F63" t="s">
+      <c r="K62" t="s">
+        <v>302</v>
+      </c>
+      <c r="L62" s="37" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="63" spans="7:12" ht="19">
+      <c r="I63" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="64" spans="4:6">
-      <c r="F64" t="s">
+      <c r="K63" t="s">
+        <v>303</v>
+      </c>
+      <c r="L63" s="37" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="64" spans="7:12" ht="19">
+      <c r="I64" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="65" spans="6:6">
-      <c r="F65" t="s">
+      <c r="K64" t="s">
+        <v>304</v>
+      </c>
+      <c r="L64" s="37" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="65" spans="9:12" ht="19">
+      <c r="I65" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="66" spans="6:6">
-      <c r="F66" t="s">
+      <c r="K65" t="s">
+        <v>305</v>
+      </c>
+      <c r="L65" s="37" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="66" spans="9:12" ht="19">
+      <c r="I66" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="67" spans="6:6">
-      <c r="F67" t="s">
+      <c r="K66" t="s">
+        <v>306</v>
+      </c>
+      <c r="L66" s="37" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="67" spans="9:12" ht="19">
+      <c r="I67" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="68" spans="6:6">
-      <c r="F68" t="s">
+      <c r="K67" t="s">
+        <v>307</v>
+      </c>
+      <c r="L67" s="37" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="68" spans="9:12" ht="19">
+      <c r="I68" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="69" spans="6:6">
-      <c r="F69" t="s">
+      <c r="K68" t="s">
+        <v>308</v>
+      </c>
+      <c r="L68" s="37" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="69" spans="9:12" ht="19">
+      <c r="I69" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="70" spans="6:6">
-      <c r="F70" t="s">
+      <c r="K69" t="s">
+        <v>309</v>
+      </c>
+      <c r="L69" s="37" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="70" spans="9:12" ht="19">
+      <c r="I70" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="71" spans="6:6">
-      <c r="F71" t="s">
+      <c r="K70" t="s">
+        <v>310</v>
+      </c>
+      <c r="L70" s="37" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="71" spans="9:12" ht="19">
+      <c r="I71" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="72" spans="6:6">
-      <c r="F72" t="s">
+      <c r="K71" t="s">
+        <v>311</v>
+      </c>
+      <c r="L71" s="37" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="72" spans="9:12" ht="19">
+      <c r="I72" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="73" spans="6:6">
-      <c r="F73" t="s">
+      <c r="K72" t="s">
+        <v>312</v>
+      </c>
+      <c r="L72" s="37" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="73" spans="9:12" ht="19">
+      <c r="I73" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="74" spans="6:6">
-      <c r="F74" t="s">
+      <c r="K73" s="40" t="s">
+        <v>314</v>
+      </c>
+      <c r="L73" s="37" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="74" spans="9:12" ht="19">
+      <c r="I74" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="75" spans="6:6">
-      <c r="F75" t="s">
+      <c r="L74" s="37" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="75" spans="9:12" ht="19">
+      <c r="I75" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="76" spans="6:6">
-      <c r="F76" t="s">
+      <c r="L75" s="37" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="76" spans="9:12" ht="19">
+      <c r="I76" t="s">
         <v>182</v>
+      </c>
+      <c r="L76" s="37" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="77" spans="9:12" ht="19">
+      <c r="L77" s="37" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="78" spans="9:12" ht="19">
+      <c r="L78" s="37" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="79" spans="9:12" ht="19">
+      <c r="L79" s="37" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="80" spans="9:12" ht="19">
+      <c r="L80" s="37" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="81" spans="12:12" ht="19">
+      <c r="L81" s="37" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="82" spans="12:12" ht="19">
+      <c r="L82" s="37" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="83" spans="12:12" ht="19">
+      <c r="L83" s="37" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="84" spans="12:12" ht="19">
+      <c r="L84" s="37" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="85" spans="12:12" ht="19">
+      <c r="L85" s="37" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="86" spans="12:12" ht="19">
+      <c r="L86" s="37" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="87" spans="12:12" ht="19">
+      <c r="L87" s="37" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="88" spans="12:12" ht="19">
+      <c r="L88" s="37" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="89" spans="12:12" ht="19">
+      <c r="L89" s="37" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="90" spans="12:12" ht="19">
+      <c r="L90" s="37" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="91" spans="12:12" ht="19">
+      <c r="L91" s="37" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="92" spans="12:12" ht="19">
+      <c r="L92" s="37" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="93" spans="12:12" ht="19">
+      <c r="L93" s="37" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="94" spans="12:12" ht="19">
+      <c r="L94" s="37" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="95" spans="12:12" ht="19">
+      <c r="L95" s="37" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="96" spans="12:12" ht="19">
+      <c r="L96" s="37" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="97" spans="12:12" ht="19">
+      <c r="L97" s="37" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="98" spans="12:12" ht="19">
+      <c r="L98" s="37" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="99" spans="12:12" ht="19">
+      <c r="L99" s="37" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="100" spans="12:12" ht="19">
+      <c r="L100" s="37" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="101" spans="12:12" ht="19">
+      <c r="L101" s="37" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="102" spans="12:12" ht="19">
+      <c r="L102" s="37" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="103" spans="12:12" ht="19">
+      <c r="L103" s="37" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="104" spans="12:12" ht="19">
+      <c r="L104" s="37" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="105" spans="12:12" ht="19">
+      <c r="L105" s="37" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="106" spans="12:12" ht="19">
+      <c r="L106" s="37" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="107" spans="12:12" ht="19">
+      <c r="L107" s="37" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="108" spans="12:12" ht="19">
+      <c r="L108" s="37" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="109" spans="12:12" ht="19">
+      <c r="L109" s="37" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="110" spans="12:12" ht="19">
+      <c r="L110" s="37" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="111" spans="12:12" ht="19">
+      <c r="L111" s="37" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="112" spans="12:12" ht="19">
+      <c r="L112" s="37" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="113" spans="12:12" ht="19">
+      <c r="L113" s="37" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="114" spans="12:12" ht="19">
+      <c r="L114" s="37" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="115" spans="12:12" ht="19">
+      <c r="L115" s="37" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="116" spans="12:12" ht="19">
+      <c r="L116" s="37" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="117" spans="12:12" ht="19">
+      <c r="L117" s="37" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="118" spans="12:12">
+      <c r="L118" s="34" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="119" spans="12:12">
+      <c r="L119" s="34" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="120" spans="12:12">
+      <c r="L120" s="34" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="121" spans="12:12">
+      <c r="L121" s="34" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="122" spans="12:12" ht="19">
+      <c r="L122" s="37" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="123" spans="12:12" ht="19">
+      <c r="L123" s="37" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="124" spans="12:12" ht="19">
+      <c r="L124" s="37" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="125" spans="12:12" ht="19">
+      <c r="L125" s="37" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="126" spans="12:12" ht="19">
+      <c r="L126" s="37" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="127" spans="12:12" ht="19">
+      <c r="L127" s="37" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="128" spans="12:12" ht="19">
+      <c r="L128" s="37" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="129" spans="12:12" ht="19">
+      <c r="L129" s="37" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="130" spans="12:12">
+      <c r="L130" s="35" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="131" spans="12:12" ht="19">
+      <c r="L131" s="37" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="132" spans="12:12" ht="19">
+      <c r="L132" s="37" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="133" spans="12:12" ht="19">
+      <c r="L133" s="37" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="134" spans="12:12" ht="19">
+      <c r="L134" s="37" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="135" spans="12:12" ht="19">
+      <c r="L135" s="37" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="136" spans="12:12" ht="19">
+      <c r="L136" s="37" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="137" spans="12:12" ht="19">
+      <c r="L137" s="37" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="138" spans="12:12" ht="19">
+      <c r="L138" s="37" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="139" spans="12:12" ht="19">
+      <c r="L139" s="37" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="140" spans="12:12" ht="19">
+      <c r="L140" s="37" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="141" spans="12:12" ht="19">
+      <c r="L141" s="37" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="142" spans="12:12" ht="19">
+      <c r="L142" s="37" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="143" spans="12:12" ht="19">
+      <c r="L143" s="37" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="144" spans="12:12" ht="19">
+      <c r="L144" s="37" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="145" spans="12:12" ht="19">
+      <c r="L145" s="37" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="146" spans="12:12" ht="19">
+      <c r="L146" s="37" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="147" spans="12:12" ht="19">
+      <c r="L147" s="37" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="148" spans="12:12" ht="19">
+      <c r="L148" s="37" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="149" spans="12:12" ht="19">
+      <c r="L149" s="37" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="150" spans="12:12" ht="19">
+      <c r="L150" s="37" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="151" spans="12:12" ht="19">
+      <c r="L151" s="37" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="152" spans="12:12" ht="19">
+      <c r="L152" s="37" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="153" spans="12:12" ht="19">
+      <c r="L153" s="37" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="154" spans="12:12" ht="19">
+      <c r="L154" s="37" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="155" spans="12:12" ht="19">
+      <c r="L155" s="37" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="156" spans="12:12" ht="19">
+      <c r="L156" s="37" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="157" spans="12:12" ht="19">
+      <c r="L157" s="37" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="158" spans="12:12" ht="19">
+      <c r="L158" s="37" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="159" spans="12:12" ht="19">
+      <c r="L159" s="37" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="160" spans="12:12" ht="19">
+      <c r="L160" s="37" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="161" spans="12:12" ht="19">
+      <c r="L161" s="37" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="162" spans="12:12" ht="19">
+      <c r="L162" s="37" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="163" spans="12:12" ht="19">
+      <c r="L163" s="37" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="164" spans="12:12" ht="19">
+      <c r="L164" s="37" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="165" spans="12:12" ht="19">
+      <c r="L165" s="37" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="166" spans="12:12" ht="19">
+      <c r="L166" s="37" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="167" spans="12:12" ht="19">
+      <c r="L167" s="37" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="168" spans="12:12" ht="19">
+      <c r="L168" s="37" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="169" spans="12:12" ht="19">
+      <c r="L169" s="37" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="170" spans="12:12">
+      <c r="L170" s="31" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="171" spans="12:12" ht="19">
+      <c r="L171" s="37" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="172" spans="12:12" ht="19">
+      <c r="L172" s="37" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="173" spans="12:12" ht="19">
+      <c r="L173" s="37" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="174" spans="12:12" ht="19">
+      <c r="L174" s="37" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="175" spans="12:12" ht="19">
+      <c r="L175" s="37" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="176" spans="12:12" ht="19">
+      <c r="L176" s="37" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="177" spans="12:12" ht="19">
+      <c r="L177" s="37" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="178" spans="12:12" ht="19">
+      <c r="L178" s="37" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="179" spans="12:12" ht="19">
+      <c r="L179" s="37" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="180" spans="12:12" ht="19">
+      <c r="L180" s="37" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="181" spans="12:12" ht="19">
+      <c r="L181" s="37" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="182" spans="12:12" ht="19">
+      <c r="L182" s="37" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="183" spans="12:12" ht="19">
+      <c r="L183" s="37" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="184" spans="12:12" ht="19">
+      <c r="L184" s="37" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="185" spans="12:12" ht="19">
+      <c r="L185" s="37" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="186" spans="12:12" ht="19">
+      <c r="L186" s="37" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="187" spans="12:12" ht="19">
+      <c r="L187" s="37" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="188" spans="12:12" ht="19">
+      <c r="L188" s="37" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="189" spans="12:12" ht="19">
+      <c r="L189" s="37" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="190" spans="12:12" ht="19">
+      <c r="L190" s="37" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="191" spans="12:12" ht="19">
+      <c r="L191" s="37" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="192" spans="12:12" ht="19">
+      <c r="L192" s="37" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="193" spans="12:12" ht="19">
+      <c r="L193" s="37" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="194" spans="12:12" ht="19">
+      <c r="L194" s="37" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="195" spans="12:12" ht="19">
+      <c r="L195" s="37" t="s">
+        <v>507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>